<commit_message>
fixed range slider dates
</commit_message>
<xml_diff>
--- a/FacebookPosts2022.xlsx
+++ b/FacebookPosts2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tasha/Desktop/NPLF-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DE6AF7-2A56-AD4D-A69A-4310F3237009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DDC17B-439C-AE4C-8952-99A7A69F7559}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{5784B273-8BFF-2245-95C6-DD3D21B91097}"/>
   </bookViews>
@@ -131,9 +131,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +148,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,10 +183,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,15 +504,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B3040F-17F5-684F-9333-FF3EFA385A3E}">
-  <dimension ref="A1:AH175"/>
+  <dimension ref="A1:AK175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:AK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,49 +616,717 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G2" s="3">
+        <v>44307</v>
+      </c>
+      <c r="I2" s="4">
+        <v>640</v>
+      </c>
+      <c r="J2" s="4">
+        <v>640</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>699</v>
+      </c>
+      <c r="M2" s="4">
+        <v>699</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <v>111</v>
+      </c>
+      <c r="P2" s="4">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>106</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0</v>
+      </c>
+      <c r="S2" s="4">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4">
+        <v>234</v>
+      </c>
+      <c r="U2" s="4">
+        <v>215</v>
+      </c>
+      <c r="V2" s="4">
+        <v>0</v>
+      </c>
+      <c r="W2" s="4">
+        <v>0</v>
+      </c>
+      <c r="X2" s="4">
+        <v>19</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G3" s="3">
+        <v>44306</v>
+      </c>
+      <c r="I3" s="4">
+        <v>151</v>
+      </c>
+      <c r="J3" s="4">
+        <v>151</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>160</v>
+      </c>
+      <c r="M3" s="4">
+        <v>160</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>5</v>
+      </c>
+      <c r="P3" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>1</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0</v>
+      </c>
+      <c r="T3" s="4">
+        <v>148</v>
+      </c>
+      <c r="U3" s="4">
+        <v>141</v>
+      </c>
+      <c r="V3" s="4">
+        <v>0</v>
+      </c>
+      <c r="W3" s="4">
+        <v>0</v>
+      </c>
+      <c r="X3" s="4">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G4" s="3">
+        <v>44306</v>
+      </c>
+      <c r="I4" s="4">
+        <v>203</v>
+      </c>
+      <c r="J4" s="4">
+        <v>203</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>213</v>
+      </c>
+      <c r="M4" s="4">
+        <v>213</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>7</v>
+      </c>
+      <c r="P4" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>3</v>
+      </c>
+      <c r="R4" s="4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4">
+        <v>117</v>
+      </c>
+      <c r="U4" s="4">
+        <v>107</v>
+      </c>
+      <c r="V4" s="4">
+        <v>0</v>
+      </c>
+      <c r="W4" s="4">
+        <v>0</v>
+      </c>
+      <c r="X4" s="4">
+        <v>5</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G5" s="3">
+        <v>44306</v>
+      </c>
+      <c r="I5" s="4">
+        <v>190</v>
+      </c>
+      <c r="J5" s="4">
+        <v>190</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>209</v>
+      </c>
+      <c r="M5" s="4">
+        <v>209</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>17</v>
+      </c>
+      <c r="P5" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>3</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0</v>
+      </c>
+      <c r="T5" s="4">
+        <v>187</v>
+      </c>
+      <c r="U5" s="4">
+        <v>174</v>
+      </c>
+      <c r="V5" s="4">
+        <v>0</v>
+      </c>
+      <c r="W5" s="4">
+        <v>0</v>
+      </c>
+      <c r="X5" s="4">
+        <v>16</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G6" s="3">
+        <v>44303</v>
+      </c>
+      <c r="I6" s="4">
+        <v>179</v>
+      </c>
+      <c r="J6" s="4">
+        <v>179</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>189</v>
+      </c>
+      <c r="M6" s="4">
+        <v>189</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>8</v>
+      </c>
+      <c r="P6" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>1</v>
+      </c>
+      <c r="R6" s="4">
+        <v>0</v>
+      </c>
+      <c r="S6" s="4">
+        <v>0</v>
+      </c>
+      <c r="T6" s="4">
+        <v>119</v>
+      </c>
+      <c r="U6" s="4">
+        <v>112</v>
+      </c>
+      <c r="V6" s="4">
+        <v>0</v>
+      </c>
+      <c r="W6" s="4">
+        <v>0</v>
+      </c>
+      <c r="X6" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G7" s="3">
+        <v>44302</v>
+      </c>
+      <c r="I7" s="4">
+        <v>179</v>
+      </c>
+      <c r="J7" s="4">
+        <v>179</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>187</v>
+      </c>
+      <c r="M7" s="4">
+        <v>187</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>15</v>
+      </c>
+      <c r="P7" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>16</v>
+      </c>
+      <c r="R7" s="4">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0</v>
+      </c>
+      <c r="T7" s="4">
+        <v>177</v>
+      </c>
+      <c r="U7" s="4">
+        <v>169</v>
+      </c>
+      <c r="V7" s="4">
+        <v>0</v>
+      </c>
+      <c r="W7" s="4">
+        <v>0</v>
+      </c>
+      <c r="X7" s="4">
+        <v>12</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G8" s="3">
+        <v>44301</v>
+      </c>
+      <c r="I8" s="4">
+        <v>97</v>
+      </c>
+      <c r="J8" s="4">
+        <v>97</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>105</v>
+      </c>
+      <c r="M8" s="4">
+        <v>105</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>5</v>
+      </c>
+      <c r="P8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0</v>
+      </c>
+      <c r="T8" s="4">
+        <v>100</v>
+      </c>
+      <c r="U8" s="4">
+        <v>92</v>
+      </c>
+      <c r="V8" s="4">
+        <v>0</v>
+      </c>
+      <c r="W8" s="4">
+        <v>0</v>
+      </c>
+      <c r="X8" s="4">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="5"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="5"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G9" s="3">
+        <v>44296</v>
+      </c>
+      <c r="I9" s="4">
+        <v>215</v>
+      </c>
+      <c r="J9" s="4">
+        <v>215</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>224</v>
+      </c>
+      <c r="M9" s="4">
+        <v>224</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>7</v>
+      </c>
+      <c r="P9" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>2</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0</v>
+      </c>
+      <c r="T9" s="4">
+        <v>87</v>
+      </c>
+      <c r="U9" s="4">
+        <v>81</v>
+      </c>
+      <c r="V9" s="4">
+        <v>0</v>
+      </c>
+      <c r="W9" s="4">
+        <v>0</v>
+      </c>
+      <c r="X9" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="5"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G10" s="3">
+        <v>44296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G11" s="3">
+        <v>44287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.2">

</xml_diff>